<commit_message>
Comienzo analisis efecto Fotoelectrico
</commit_message>
<xml_diff>
--- a/Bloque Cuantica-Estadistica/P1B Fotoelectrico/P1B.xlsx
+++ b/Bloque Cuantica-Estadistica/P1B Fotoelectrico/P1B.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feyra\Desktop\UNI\T-cnicas-experimentales-II\Bloque Cuantica-Estadistica\P1B Fotoelectrico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B6343E-0440-4ED4-B80E-6F4EC12EAAD7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EDC8FBE-353E-45B4-8DAC-8DBA7BC9321B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parte 1" sheetId="1" r:id="rId1"/>
@@ -13372,8 +13372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:F114"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="D98" sqref="D98:E114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13871,11 +13871,11 @@
         <v>13.5</v>
       </c>
       <c r="C33" s="3">
-        <f t="shared" ref="C33:C56" si="3">$A$4/$A$6* SIN(B33 * PI()/180)</f>
+        <f t="shared" ref="C33:C42" si="3">$A$4/$A$6* SIN(B33 * PI()/180)</f>
         <v>389.07560642650901</v>
       </c>
       <c r="D33" s="4">
-        <f t="shared" ref="D33:D56" si="4">2.99792*10^8 /(C33*10^-9)</f>
+        <f t="shared" ref="D33:D42" si="4">2.99792*10^8 /(C33*10^-9)</f>
         <v>770523762086910.88</v>
       </c>
       <c r="E33">
@@ -14597,8 +14597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{556F8399-813B-44D5-9B7B-7CC36300CE37}">
   <dimension ref="B1:R64"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3:R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14791,7 +14791,7 @@
         <v>5.3</v>
       </c>
       <c r="K5">
-        <f t="shared" ref="K5:K13" si="3">K4+0.01</f>
+        <f t="shared" ref="K5:K12" si="3">K4+0.01</f>
         <v>0.42000000000000004</v>
       </c>
       <c r="L5">
@@ -15269,8 +15269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ADBD9F1-5668-4CC2-8E1F-5A4946D09955}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>